<commit_message>
Added initIR and readIR
</commit_message>
<xml_diff>
--- a/taobao.xlsx
+++ b/taobao.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\senrcjlw2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7A49E4-9BED-4079-BDC2-3FE33E251AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F2D82F-5991-44A8-A9B8-FA56607CC930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{B6413BF9-0226-4B9D-AF3F-9640BE578E9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{B6413BF9-0226-4B9D-AF3F-9640BE578E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Layer 3 LW SEN" sheetId="1" r:id="rId1"/>
     <sheet name="Layer 2 LW SEN" sheetId="2" r:id="rId2"/>
+    <sheet name="Layer 1 LW SEN" sheetId="3" r:id="rId3"/>
+    <sheet name="Combined" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Layer 3 LW SEN'!$1:$1</definedName>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>Comment</t>
   </si>
@@ -87,12 +89,6 @@
     <t>LED 0603</t>
   </si>
   <si>
-    <t>MTH</t>
-  </si>
-  <si>
-    <t>m3 Mouting Hole</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -105,12 +101,6 @@
     <t>RES 1K 0603</t>
   </si>
   <si>
-    <t>470</t>
-  </si>
-  <si>
-    <t>RES 470 0603</t>
-  </si>
-  <si>
     <t>STM32F103CBT6</t>
   </si>
   <si>
@@ -150,9 +140,6 @@
     <t>https://item.taobao.com/item.htm?spm=a1z09.2.0.0.34fc2e8dHwwdXv&amp;id=607466949581&amp;_u=k30vu5iqe6af</t>
   </si>
   <si>
-    <t>NIL</t>
-  </si>
-  <si>
     <t>https://item.taobao.com/item.htm?spm=a1z09.2.0.0.34fc2e8dHwwdXv&amp;id=525777943950&amp;_u=k30vu5iq2d08</t>
   </si>
   <si>
@@ -165,15 +152,6 @@
     <t>https://item.taobao.com/item.htm?spm=2013.1.0.0.33151207fEsB13&amp;id=565792478624 (1), https://item.taobao.com/item.htm?spm=2013.1.0.0.7f38691fADzce1&amp;id=565715285795(2)</t>
   </si>
   <si>
-    <t>No stock probably using 16mhz</t>
-  </si>
-  <si>
-    <t>OPENMV3</t>
-  </si>
-  <si>
-    <t>Camera</t>
-  </si>
-  <si>
     <t>10nF</t>
   </si>
   <si>
@@ -208,18 +186,6 @@
   </si>
   <si>
     <t>Diode</t>
-  </si>
-  <si>
-    <t>CONN_04LOCK</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>CONN_03LOCK</t>
-  </si>
-  <si>
-    <t>14AWG</t>
   </si>
   <si>
     <t>11 Pin Vertical Molex</t>
@@ -652,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF0C792-AC26-48B8-B839-288C2CA2D6E5}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,215 +643,187 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
       <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1">
-        <v>4</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{90463267-F493-48AE-AC62-653D79542D28}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{9B1F248C-98A3-4AB9-83C0-346FB8DF203F}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{7C8D6DC5-3DBB-450D-8A6F-8F005551505B}"/>
-    <hyperlink ref="D3" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a1z0d.6639537/tb.1997196601.28.42ef7484KnHHst&amp;id=624642040106" xr:uid="{8BCE800E-CA1B-471E-A8AB-34AA277CF4CF}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{CBDAAD92-B957-4EC6-BD34-5BE99B7A77CF}"/>
-    <hyperlink ref="D2" r:id="rId6" xr:uid="{84205971-D33F-4731-8BFE-DD370C032713}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{A0E0588D-8E62-4DB8-A775-F53DD5FEE527}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{6147ABDC-6148-46B7-882A-B6D07C44A23B}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{9965C3CC-F19A-4F58-B4B1-9971B1D0413E}"/>
-    <hyperlink ref="D14" r:id="rId10" display="https://item.taobao.com/item.htm?spm=2013.1.0.0.33151207fEsB13&amp;id=565792478624" xr:uid="{A26FFC6D-4220-457D-998C-A412DDF9359E}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{90463267-F493-48AE-AC62-653D79542D28}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{9B1F248C-98A3-4AB9-83C0-346FB8DF203F}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{7C8D6DC5-3DBB-450D-8A6F-8F005551505B}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{CBDAAD92-B957-4EC6-BD34-5BE99B7A77CF}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{84205971-D33F-4731-8BFE-DD370C032713}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{A0E0588D-8E62-4DB8-A775-F53DD5FEE527}"/>
+    <hyperlink ref="D2" r:id="rId7" xr:uid="{6147ABDC-6148-46B7-882A-B6D07C44A23B}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{9965C3CC-F19A-4F58-B4B1-9971B1D0413E}"/>
+    <hyperlink ref="D11" r:id="rId9" display="https://item.taobao.com/item.htm?spm=2013.1.0.0.33151207fEsB13&amp;id=565792478624" xr:uid="{A26FFC6D-4220-457D-998C-A412DDF9359E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72A6527-01BA-4430-9C24-3E02F97DDFF6}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,54 +845,54 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -962,32 +900,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -995,32 +933,32 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -1028,54 +966,54 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1083,148 +1021,109 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+    <sortCondition ref="A2:A24"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18A77C-247B-474F-86CA-DDA8E112815B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C09B171-6ECF-40A9-8E5E-47AF01B45B90}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>